<commit_message>
Add CPU-only PyTorch, Render deployment config, job title filter & date fix
</commit_message>
<xml_diff>
--- a/Company list.xlsx
+++ b/Company list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darji\OneDrive\Desktop\JobFinder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1240fc7f40621c75/Desktop/JobFinder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9E9EC3-CC87-411C-A51D-FF0A98EF5F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{CE9E9EC3-CC87-411C-A51D-FF0A98EF5F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69064492-5524-4014-8A6A-E1CF69DF0BDA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A880259E-2144-3049-BB67-23F9B36A6CBC}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{A880259E-2144-3049-BB67-23F9B36A6CBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Adobe</t>
   </si>
@@ -211,6 +211,36 @@
   </si>
   <si>
     <t>Comcast</t>
+  </si>
+  <si>
+    <t>https://sonyglobal.wd1.myworkdayjobs.com/en-US/SonyGlobalCareers/</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>https://nike.wd1.myworkdayjobs.com/nke/</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>https://thehartford.wd5.myworkdayjobs.com/en-US/Careers_External</t>
+  </si>
+  <si>
+    <t>The Hartford</t>
+  </si>
+  <si>
+    <t>https://keystone.wd5.myworkdayjobs.com/Keystone/</t>
+  </si>
+  <si>
+    <t>Keystone</t>
+  </si>
+  <si>
+    <t>https://therapybrands.wd1.myworkdayjobs.com/EnsoraHealth</t>
+  </si>
+  <si>
+    <t>EnsoraHealth</t>
   </si>
 </sst>
 </file>
@@ -253,10 +283,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8291B39E-7C11-2645-9F9A-A91128E0C79A}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -728,7 +757,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
@@ -736,7 +765,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
@@ -744,7 +773,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
@@ -752,7 +781,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
       <c r="B18" t="s">
@@ -760,7 +789,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>40</v>
       </c>
       <c r="B19" t="s">
@@ -768,7 +797,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>42</v>
       </c>
       <c r="B20" t="s">
@@ -776,7 +805,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>44</v>
       </c>
       <c r="B21" t="s">
@@ -784,7 +813,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
       <c r="B22" t="s">
@@ -792,7 +821,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
@@ -800,7 +829,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="B24" t="s">
@@ -808,7 +837,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
       <c r="B25" t="s">
@@ -816,7 +845,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>54</v>
       </c>
       <c r="B26" t="s">
@@ -824,7 +853,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>56</v>
       </c>
       <c r="B27" t="s">
@@ -832,7 +861,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
       <c r="B28" t="s">
@@ -840,16 +869,44 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
+      <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>